<commit_message>
add NCREE2011 in GMPEhaz.model list
</commit_message>
<xml_diff>
--- a/data-raw/GMPE_list.xlsx
+++ b/data-raw/GMPE_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\Rwork\TD15014\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\GMPEhaz\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="161">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -600,6 +600,18 @@
   </si>
   <si>
     <t>LL08_F04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NCREE2011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NCREE_2011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taiwan</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -933,11 +945,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3106,10 +3118,10 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>158</v>
       </c>
       <c r="B58" t="s">
-        <v>118</v>
+        <v>159</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -3121,13 +3133,13 @@
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>71</v>
+        <v>160</v>
       </c>
       <c r="G58">
         <v>1</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58">
         <v>0</v>
@@ -3139,15 +3151,15 @@
         <v>0.01</v>
       </c>
       <c r="L58">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>150</v>
+        <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -3159,7 +3171,7 @@
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -3182,22 +3194,22 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -3220,10 +3232,10 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -3235,7 +3247,7 @@
         <v>1</v>
       </c>
       <c r="F61" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -3258,19 +3270,19 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62" t="s">
         <v>59</v>
@@ -3291,30 +3303,30 @@
         <v>0.01</v>
       </c>
       <c r="L62">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H63">
         <v>1</v>
@@ -3326,18 +3338,18 @@
         <v>0</v>
       </c>
       <c r="K63">
-        <v>7.4999999999999997E-2</v>
+        <v>0.01</v>
       </c>
       <c r="L63">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B64" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -3367,18 +3379,18 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L64">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -3387,7 +3399,7 @@
         <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -3402,27 +3414,27 @@
         <v>0</v>
       </c>
       <c r="K65">
-        <v>0.01</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="L65">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F66" t="s">
         <v>62</v>
@@ -3448,16 +3460,16 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -3486,19 +3498,19 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" t="s">
         <v>62</v>
@@ -3522,18 +3534,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="33" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>50</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>127</v>
+        <v>49</v>
+      </c>
+      <c r="B69" t="s">
+        <v>126</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -3557,6 +3569,44 @@
         <v>0.01</v>
       </c>
       <c r="L69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="33" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>50</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
+        <v>62</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>0.01</v>
+      </c>
+      <c r="L70">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update GMPEhaz-model from GMPE_list.xlsx
</commit_message>
<xml_diff>
--- a/data-raw/GMPE_list.xlsx
+++ b/data-raw/GMPE_list.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="166">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>ASK14.tw.C01</t>
-  </si>
-  <si>
-    <t>BCHydroSubV3</t>
   </si>
   <si>
     <t>BI14</t>
@@ -612,6 +609,28 @@
   </si>
   <si>
     <t>Taiwan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCHydroSubV3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCHydroSub2018Global</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCHydroSub2018SouthAM</t>
+  </si>
+  <si>
+    <t>BCHydroSub2018TW</t>
+  </si>
+  <si>
+    <t>Global</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SouthAM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -945,16 +964,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
+      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.25" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.625" customWidth="1"/>
@@ -967,37 +986,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
         <v>78</v>
       </c>
-      <c r="I1" t="s">
-        <v>79</v>
-      </c>
       <c r="J1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
         <v>65</v>
-      </c>
-      <c r="L1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1005,7 +1024,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1017,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1043,7 +1062,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1055,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1081,7 +1100,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1093,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1116,11 +1135,11 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
         <v>131</v>
       </c>
-      <c r="B5" t="s">
-        <v>132</v>
-      </c>
       <c r="C5">
         <v>0</v>
       </c>
@@ -1131,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1157,7 +1176,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1169,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1195,7 +1214,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1207,7 +1226,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1233,7 +1252,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1245,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1268,10 +1287,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1283,7 +1302,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1309,7 +1328,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1321,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1344,11 +1363,11 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" t="s">
         <v>133</v>
       </c>
-      <c r="B11" t="s">
-        <v>134</v>
-      </c>
       <c r="C11">
         <v>1</v>
       </c>
@@ -1359,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1385,7 +1404,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1397,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1423,7 +1442,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1435,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1461,7 +1480,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1473,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1496,11 +1515,11 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" t="s">
         <v>135</v>
       </c>
-      <c r="B15" t="s">
-        <v>136</v>
-      </c>
       <c r="C15">
         <v>1</v>
       </c>
@@ -1511,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1534,10 +1553,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1549,7 +1568,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1572,22 +1591,22 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>161</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>164</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1596,39 +1615,39 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="L17">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>162</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>165</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1640,30 +1659,30 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="L18">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>163</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1678,18 +1697,18 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="L19">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1701,16 +1720,16 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -1724,10 +1743,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1739,16 +1758,16 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -1757,15 +1776,15 @@
         <v>0.01</v>
       </c>
       <c r="L21">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1777,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1795,15 +1814,15 @@
         <v>0.01</v>
       </c>
       <c r="L22">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1815,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1833,15 +1852,15 @@
         <v>0.01</v>
       </c>
       <c r="L23">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1853,16 +1872,16 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -1876,10 +1895,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1891,10 +1910,10 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -1906,18 +1925,18 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="L25">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1929,16 +1948,16 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <v>1</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -1952,10 +1971,10 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>138</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1967,7 +1986,7 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1990,10 +2009,10 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>155</v>
+        <v>97</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2005,10 +2024,10 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -2020,68 +2039,68 @@
         <v>0</v>
       </c>
       <c r="K28">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="L28">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29">
         <v>0.01</v>
       </c>
       <c r="L29">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>82</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -2093,21 +2112,21 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K30">
         <v>0.01</v>
       </c>
       <c r="L30">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>153</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2119,16 +2138,16 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -2142,25 +2161,25 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -2169,33 +2188,33 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32">
         <v>0.01</v>
       </c>
       <c r="L32">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>140</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -2207,21 +2226,21 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33">
         <v>0.01</v>
       </c>
       <c r="L33">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2233,16 +2252,16 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -2256,10 +2275,10 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2271,10 +2290,10 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -2294,25 +2313,25 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -2324,18 +2343,18 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="L36">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2347,10 +2366,10 @@
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -2370,25 +2389,25 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>142</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -2400,30 +2419,30 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="L38">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -2438,18 +2457,18 @@
         <v>0</v>
       </c>
       <c r="K39">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="L39">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2461,10 +2480,10 @@
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -2484,25 +2503,25 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -2514,18 +2533,18 @@
         <v>0</v>
       </c>
       <c r="K41">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="L41">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2537,10 +2556,10 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -2560,10 +2579,10 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2575,16 +2594,16 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -2593,30 +2612,30 @@
         <v>0.01</v>
       </c>
       <c r="L43">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -2628,18 +2647,18 @@
         <v>0</v>
       </c>
       <c r="K44">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="L44">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2651,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -2669,12 +2688,15 @@
         <v>0.01</v>
       </c>
       <c r="L45">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="B46" t="s">
+        <v>108</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -2686,16 +2708,16 @@
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -2704,30 +2726,30 @@
         <v>0.01</v>
       </c>
       <c r="L46">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="33" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>112</v>
+        <v>32</v>
+      </c>
+      <c r="B47" t="s">
+        <v>109</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -2739,18 +2761,18 @@
         <v>0</v>
       </c>
       <c r="K47">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="L47">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="33" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>37</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>113</v>
+        <v>33</v>
+      </c>
+      <c r="B48" t="s">
+        <v>110</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -2762,7 +2784,7 @@
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -2785,19 +2807,19 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -2818,24 +2840,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>130</v>
-      </c>
-      <c r="B50" t="s">
-        <v>128</v>
+        <v>35</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -2856,24 +2878,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="33" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>147</v>
-      </c>
-      <c r="B51" t="s">
-        <v>149</v>
+        <v>36</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -2896,10 +2918,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>156</v>
-      </c>
-      <c r="B52" t="s">
-        <v>157</v>
+        <v>37</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2911,7 +2930,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -2934,10 +2953,10 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="B53" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2949,7 +2968,7 @@
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -2972,10 +2991,10 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="B54" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -2987,7 +3006,7 @@
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G54">
         <v>1</v>
@@ -3010,22 +3029,22 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>155</v>
       </c>
       <c r="B55" t="s">
-        <v>115</v>
+        <v>156</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -3038,14 +3057,20 @@
       </c>
       <c r="J55">
         <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0.01</v>
+      </c>
+      <c r="L55">
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -3057,10 +3082,10 @@
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -3072,18 +3097,18 @@
         <v>0</v>
       </c>
       <c r="K56">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="L56">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -3095,10 +3120,10 @@
         <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -3113,15 +3138,15 @@
         <v>0.01</v>
       </c>
       <c r="L57">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>158</v>
+        <v>40</v>
       </c>
       <c r="B58" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -3133,48 +3158,42 @@
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>160</v>
+        <v>58</v>
       </c>
       <c r="G58">
         <v>1</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58">
         <v>0</v>
       </c>
       <c r="J58">
         <v>0</v>
-      </c>
-      <c r="K58">
-        <v>0.01</v>
-      </c>
-      <c r="L58">
-        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -3186,33 +3205,33 @@
         <v>0</v>
       </c>
       <c r="K59">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="L59">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="B60" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -3227,33 +3246,33 @@
         <v>0.01</v>
       </c>
       <c r="L60">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>157</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>158</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>72</v>
+        <v>159</v>
       </c>
       <c r="G61">
         <v>1</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -3265,27 +3284,27 @@
         <v>0.01</v>
       </c>
       <c r="L61">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -3308,10 +3327,10 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>149</v>
       </c>
       <c r="B63" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -3323,7 +3342,7 @@
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G63">
         <v>1</v>
@@ -3341,15 +3360,15 @@
         <v>0.01</v>
       </c>
       <c r="L63">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -3361,10 +3380,10 @@
         <v>1</v>
       </c>
       <c r="F64" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -3376,18 +3395,18 @@
         <v>0</v>
       </c>
       <c r="K64">
-        <v>7.4999999999999997E-2</v>
+        <v>0.01</v>
       </c>
       <c r="L64">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>45</v>
+        <v>151</v>
       </c>
       <c r="B65" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -3399,10 +3418,10 @@
         <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -3414,33 +3433,33 @@
         <v>0</v>
       </c>
       <c r="K65">
-        <v>7.4999999999999997E-2</v>
+        <v>0.01</v>
       </c>
       <c r="L65">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -3455,27 +3474,27 @@
         <v>0.01</v>
       </c>
       <c r="L66">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B67" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -3490,18 +3509,18 @@
         <v>0</v>
       </c>
       <c r="K67">
-        <v>0.01</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="L67">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B68" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -3510,10 +3529,10 @@
         <v>1</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -3528,30 +3547,30 @@
         <v>0</v>
       </c>
       <c r="K68">
-        <v>0.01</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="L68">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B69" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69">
         <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -3572,24 +3591,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="33" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>50</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>127</v>
+        <v>46</v>
+      </c>
+      <c r="B70" t="s">
+        <v>123</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -3607,6 +3626,120 @@
         <v>0.01</v>
       </c>
       <c r="L70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>47</v>
+      </c>
+      <c r="B71" t="s">
+        <v>124</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>61</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0.01</v>
+      </c>
+      <c r="L71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>48</v>
+      </c>
+      <c r="B72" t="s">
+        <v>125</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
+        <v>61</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0.01</v>
+      </c>
+      <c r="L72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="33" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>49</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" t="s">
+        <v>61</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0.01</v>
+      </c>
+      <c r="L73">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update max period of BSSA14.tw.E02 in GMPE_list
</commit_message>
<xml_diff>
--- a/data-raw/GMPE_list.xlsx
+++ b/data-raw/GMPE_list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\GMPEhaz\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/person/Git/GMPEhaz/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1385AB-9050-FF43-922A-66567D4399BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -637,8 +638,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -963,25 +964,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomLeft" activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1019,7 +1020,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1057,7 +1058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1095,7 +1096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1133,7 +1134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -1171,7 +1172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1209,7 +1210,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1247,7 +1248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1285,7 +1286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -1323,7 +1324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1361,7 +1362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -1399,7 +1400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1437,7 +1438,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1475,7 +1476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1513,7 +1514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>134</v>
       </c>
@@ -1551,7 +1552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -1589,7 +1590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>161</v>
       </c>
@@ -1627,7 +1628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>162</v>
       </c>
@@ -1665,7 +1666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>163</v>
       </c>
@@ -1703,7 +1704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1741,7 +1742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1779,7 +1780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1817,7 +1818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>136</v>
       </c>
@@ -1855,7 +1856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1893,7 +1894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1931,7 +1932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1969,7 +1970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>138</v>
       </c>
@@ -2004,10 +2005,10 @@
         <v>0.01</v>
       </c>
       <c r="L27">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -2045,7 +2046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -2083,7 +2084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -2121,7 +2122,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>153</v>
       </c>
@@ -2159,7 +2160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -2235,7 +2236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -2273,7 +2274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2311,7 +2312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>23</v>
       </c>
@@ -2349,7 +2350,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -2387,7 +2388,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>142</v>
       </c>
@@ -2425,7 +2426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -2463,7 +2464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -2501,7 +2502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>27</v>
       </c>
@@ -2539,7 +2540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>28</v>
       </c>
@@ -2577,7 +2578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>29</v>
       </c>
@@ -2615,7 +2616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -2653,7 +2654,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>144</v>
       </c>
@@ -2691,7 +2692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -2729,7 +2730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
         <v>32</v>
       </c>
@@ -2767,7 +2768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -2840,7 +2841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="33" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="32">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -2878,7 +2879,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="33" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="32">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -2916,7 +2917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -2951,7 +2952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>129</v>
       </c>
@@ -2989,7 +2990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>146</v>
       </c>
@@ -3027,7 +3028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
         <v>155</v>
       </c>
@@ -3065,7 +3066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -3103,7 +3104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>39</v>
       </c>
@@ -3141,7 +3142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
         <v>40</v>
       </c>
@@ -3173,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
         <v>41</v>
       </c>
@@ -3211,7 +3212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
         <v>42</v>
       </c>
@@ -3249,7 +3250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
         <v>157</v>
       </c>
@@ -3287,7 +3288,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -3325,7 +3326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>149</v>
       </c>
@@ -3363,7 +3364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -3401,7 +3402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>151</v>
       </c>
@@ -3439,7 +3440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -3477,7 +3478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>43</v>
       </c>
@@ -3515,7 +3516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>44</v>
       </c>
@@ -3553,7 +3554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>45</v>
       </c>
@@ -3591,7 +3592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
         <v>46</v>
       </c>
@@ -3629,7 +3630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>47</v>
       </c>
@@ -3667,7 +3668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -3705,7 +3706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="33" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="32">
       <c r="A73" t="s">
         <v>49</v>
       </c>

</xml_diff>